<commit_message>
2014 05 05   10:53
</commit_message>
<xml_diff>
--- a/BD2_2M/T4 - Trigges/Agenda de projeto.xlsx
+++ b/BD2_2M/T4 - Trigges/Agenda de projeto.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="35">
   <si>
     <t>Ação</t>
   </si>
@@ -154,9 +154,6 @@
   </si>
   <si>
     <t>T4 - Trigges</t>
-  </si>
-  <si>
-    <t>Tabela Nf</t>
   </si>
   <si>
     <t>Tabela NF</t>
@@ -1081,8 +1078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1100,7 +1097,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="15" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="28"/>
@@ -1273,7 +1270,7 @@
         <v>25</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3">
@@ -1295,7 +1292,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>31</v>
@@ -1319,7 +1316,7 @@
         <v>25</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="25"/>
       <c r="D11" s="3">

</xml_diff>

<commit_message>
2014 05 05 11:27
Agenda
</commit_message>
<xml_diff>
--- a/BD2_2M/T4 - Trigges/Agenda de projeto.xlsx
+++ b/BD2_2M/T4 - Trigges/Agenda de projeto.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="36">
   <si>
     <t>Ação</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>Atividades estão detalhadas no arquivo "BD2 Trabalho 1  TRIGGER ESTOQUE"</t>
+  </si>
+  <si>
+    <t>Trigges Controle de estoque</t>
   </si>
 </sst>
 </file>
@@ -1079,7 +1082,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1334,22 +1337,49 @@
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="3"/>
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="3">
+        <v>9</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="24"/>
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>35</v>
+      </c>
       <c r="C13" s="25"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="3"/>
+      <c r="D13" s="3">
+        <v>10</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1436,7 +1466,7 @@
       </c>
       <c r="B19" s="20">
         <f>COUNTA(B4:B18)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C19" s="12"/>
       <c r="D19" s="13"/>

</xml_diff>

<commit_message>
2014 05 12 09:35
</commit_message>
<xml_diff>
--- a/BD2_2M/T4 - Trigges/Agenda de projeto.xlsx
+++ b/BD2_2M/T4 - Trigges/Agenda de projeto.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$3:$G$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$3:$G$17</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -478,7 +478,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>200025</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -521,7 +521,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>200025</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -564,7 +564,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -607,7 +607,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -655,7 +655,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -703,7 +703,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -751,7 +751,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1079,10 +1079,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1392,91 +1392,71 @@
       <c r="G14" s="3"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="5"/>
+    <row r="15" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="3">
+        <v>29</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="3"/>
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="3">
+        <v>30</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="3">
-        <v>29</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="3">
-        <v>30</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="1:8" s="18" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="11" t="s">
+    <row r="17" spans="1:8" s="18" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="20">
-        <f>COUNTA(B4:B18)</f>
+      <c r="B17" s="20">
+        <f>COUNTA(B4:B16)</f>
         <v>12</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="14"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="14"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:G19"/>
+  <autoFilter ref="A3:G17"/>
   <mergeCells count="2">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:D2"/>

</xml_diff>

<commit_message>
2014 05 12 10:13
</commit_message>
<xml_diff>
--- a/BD2_2M/T4 - Trigges/Agenda de projeto.xlsx
+++ b/BD2_2M/T4 - Trigges/Agenda de projeto.xlsx
@@ -165,7 +165,7 @@
     <t>Atividades estão detalhadas no arquivo "BD2 Trabalho 1  TRIGGER ESTOQUE"</t>
   </si>
   <si>
-    <t>Trigges Controle de estoque</t>
+    <t>Trigges Edita produtos</t>
   </si>
 </sst>
 </file>
@@ -1082,7 +1082,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
2014 05 12 10:38
Finaliazarção do trabalho
</commit_message>
<xml_diff>
--- a/BD2_2M/T4 - Trigges/Agenda de projeto.xlsx
+++ b/BD2_2M/T4 - Trigges/Agenda de projeto.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="34">
   <si>
     <t>Ação</t>
   </si>
@@ -123,18 +123,9 @@
     <t xml:space="preserve">Estrutura da atividade </t>
   </si>
   <si>
-    <t xml:space="preserve">Todas as tabelas e funções </t>
-  </si>
-  <si>
     <t>Entrega</t>
   </si>
   <si>
-    <t>T3 - Avalicação 2014-16</t>
-  </si>
-  <si>
-    <t>T3 - Avalicação 2014-17</t>
-  </si>
-  <si>
     <t>Insert</t>
   </si>
   <si>
@@ -166,6 +157,9 @@
   </si>
   <si>
     <t>Trigges Edita produtos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Todas as tabelas e trigger </t>
   </si>
 </sst>
 </file>
@@ -1082,7 +1076,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1100,7 +1094,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="15" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="28"/>
@@ -1112,13 +1106,13 @@
     </row>
     <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
       <c r="D2" s="29"/>
       <c r="E2" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F2" s="22">
         <v>41771</v>
@@ -1162,7 +1156,7 @@
         <v>20</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D4" s="3">
         <v>1</v>
@@ -1186,7 +1180,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D5" s="3">
         <v>2</v>
@@ -1207,10 +1201,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D6" s="16">
         <v>6</v>
@@ -1222,15 +1216,15 @@
         <v>18</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D7" s="16">
         <v>6</v>
@@ -1250,10 +1244,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D8" s="16">
         <v>7</v>
@@ -1265,15 +1259,15 @@
         <v>18</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3">
@@ -1295,10 +1289,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D10" s="3">
         <v>8</v>
@@ -1310,16 +1304,16 @@
         <v>18</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C11" s="25"/>
       <c r="D11" s="3">
@@ -1341,10 +1335,10 @@
         <v>8</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D12" s="3">
         <v>9</v>
@@ -1353,10 +1347,10 @@
         <v>9</v>
       </c>
       <c r="F12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="H12" s="5"/>
     </row>
@@ -1365,7 +1359,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C13" s="25"/>
       <c r="D13" s="3">
@@ -1375,7 +1369,7 @@
         <v>10</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>14</v>
@@ -1397,10 +1391,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D15" s="3">
         <v>29</v>
@@ -1409,7 +1403,7 @@
         <v>10</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>14</v>
@@ -1424,7 +1418,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D16" s="3">
         <v>30</v>
@@ -1433,7 +1427,7 @@
         <v>9</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>17</v>

</xml_diff>